<commit_message>
Fixed req ID #
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{2DA582E0-682E-4364-A321-ED4B350B6AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E5AC12-077B-4FB4-AC5C-B8D0A500E5C5}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{2DA582E0-682E-4364-A321-ED4B350B6AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A5A7DB5-AD7B-4E03-A7EE-4FD725187B2E}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="11240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
     <t>The system shall allow the creation of a new game from two Player objects</t>
   </si>
   <si>
-    <t>GM_12</t>
+    <t>GM_3</t>
   </si>
 </sst>
 </file>
@@ -855,31 +855,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="36.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="8.85546875" style="3"/>
-    <col min="17" max="17" width="8.85546875" style="12"/>
-    <col min="18" max="18" width="8.85546875" style="3"/>
-    <col min="19" max="19" width="36.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.81640625" style="3"/>
+    <col min="2" max="2" width="36.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="8.81640625" style="3"/>
+    <col min="17" max="17" width="8.81640625" style="12"/>
+    <col min="18" max="18" width="8.81640625" style="3"/>
+    <col min="19" max="19" width="36.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F2" s="9" t="s">
         <v>49</v>
       </c>
@@ -917,7 +917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -937,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -960,7 +960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -968,27 +968,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="F24" s="10"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="F25" s="10"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1232,7 +1232,7 @@
       <c r="F26" s="10"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -1248,7 +1248,7 @@
       <c r="F27" s="10"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="F29" s="10"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1298,7 +1298,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -1362,9 +1362,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>92</v>
@@ -1376,9 +1376,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>92</v>
@@ -1390,9 +1390,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>92</v>
@@ -1404,9 +1404,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>92</v>
@@ -1418,9 +1418,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>92</v>
@@ -1432,9 +1432,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>92</v>
@@ -1446,9 +1446,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>92</v>
@@ -1460,9 +1460,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>92</v>
@@ -1474,9 +1474,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
update FinalRequirements.xlsx Team 2
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uta\SPring 2025\fundamental\projectFinal\cse3310-sp25-004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{7BE73A8F-EFB8-45D8-962F-A705BD3273A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84BC1B33-ADE7-4B30-B949-DEDA3A2E2F52}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F121F39-4C40-47D8-86E9-FDB2C932ED91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="11240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="275">
   <si>
     <t>Tested By</t>
   </si>
@@ -515,13 +515,361 @@
   </si>
   <si>
     <t>sendUpdateBoard()</t>
+  </si>
+  <si>
+    <t>T2_001</t>
+  </si>
+  <si>
+    <t>T2_002</t>
+  </si>
+  <si>
+    <t>T2_003</t>
+  </si>
+  <si>
+    <t>T2_005</t>
+  </si>
+  <si>
+    <t>T2_006</t>
+  </si>
+  <si>
+    <t>T2_007</t>
+  </si>
+  <si>
+    <t>T2_008</t>
+  </si>
+  <si>
+    <t>T2_009</t>
+  </si>
+  <si>
+    <t>T2_010</t>
+  </si>
+  <si>
+    <t>T2_011</t>
+  </si>
+  <si>
+    <t>T2_012</t>
+  </si>
+  <si>
+    <t>T2_013</t>
+  </si>
+  <si>
+    <t>T2_014</t>
+  </si>
+  <si>
+    <t>T2_015</t>
+  </si>
+  <si>
+    <t>T2_016</t>
+  </si>
+  <si>
+    <t>T2_017</t>
+  </si>
+  <si>
+    <t>T2_019</t>
+  </si>
+  <si>
+    <t>T2_020</t>
+  </si>
+  <si>
+    <t>T2_021</t>
+  </si>
+  <si>
+    <t>T2_025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2_025 </t>
+  </si>
+  <si>
+    <t>T2_026</t>
+  </si>
+  <si>
+    <t>T2_027</t>
+  </si>
+  <si>
+    <t>T2_029</t>
+  </si>
+  <si>
+    <t>T2_030</t>
+  </si>
+  <si>
+    <t>T2_031</t>
+  </si>
+  <si>
+    <t>T2_032</t>
+  </si>
+  <si>
+    <t>T2_33</t>
+  </si>
+  <si>
+    <t>T2_34</t>
+  </si>
+  <si>
+    <t>T2_35</t>
+  </si>
+  <si>
+    <t>T2_36</t>
+  </si>
+  <si>
+    <t>T2_37</t>
+  </si>
+  <si>
+    <t>T2_38</t>
+  </si>
+  <si>
+    <t>T2_39</t>
+  </si>
+  <si>
+    <t>2 - Join game</t>
+  </si>
+  <si>
+    <t>3 - Join game</t>
+  </si>
+  <si>
+    <t>4 - Join game</t>
+  </si>
+  <si>
+    <t>6 - Join game</t>
+  </si>
+  <si>
+    <t>7 - Join game</t>
+  </si>
+  <si>
+    <t>8 - Join game</t>
+  </si>
+  <si>
+    <t>9 - Join game</t>
+  </si>
+  <si>
+    <t>10 - Join game</t>
+  </si>
+  <si>
+    <t>11 - Join game</t>
+  </si>
+  <si>
+    <t>12 - Join game</t>
+  </si>
+  <si>
+    <t>13 - Join game</t>
+  </si>
+  <si>
+    <t>14 - Join game</t>
+  </si>
+  <si>
+    <t>15 - Join game</t>
+  </si>
+  <si>
+    <t>16 - Join game</t>
+  </si>
+  <si>
+    <t>17 - Join game</t>
+  </si>
+  <si>
+    <t>18 - Join game</t>
+  </si>
+  <si>
+    <t>20 - Join game</t>
+  </si>
+  <si>
+    <t>21 - Join game</t>
+  </si>
+  <si>
+    <t>22 - Join game</t>
+  </si>
+  <si>
+    <t>26 - Join game</t>
+  </si>
+  <si>
+    <t>27 - Join game</t>
+  </si>
+  <si>
+    <t>28 - Join game</t>
+  </si>
+  <si>
+    <t>29 - Join game</t>
+  </si>
+  <si>
+    <t>31 - Join game</t>
+  </si>
+  <si>
+    <t>32 - Join game</t>
+  </si>
+  <si>
+    <t>33 - Join game</t>
+  </si>
+  <si>
+    <t>34 - Join game</t>
+  </si>
+  <si>
+    <t>35 - Join game</t>
+  </si>
+  <si>
+    <t>36 - Join game</t>
+  </si>
+  <si>
+    <t>37 - Join game</t>
+  </si>
+  <si>
+    <t>38 - Join game</t>
+  </si>
+  <si>
+    <t>39 - Join game</t>
+  </si>
+  <si>
+    <t>40 - Join game</t>
+  </si>
+  <si>
+    <t>41 - Join game</t>
+  </si>
+  <si>
+    <t>Data with list of player names shall be fetched from PageManager with a list of players in String Json when a player is logged in</t>
+  </si>
+  <si>
+    <t>Data fetched from PageManager shall be parsed into JSON where a for each loop with iterate through the list of players to get the current player and call T2_33 to dyanmically add players to the html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">any event from each player shall be sent to page manager directly to transfer to other element of the game </t>
+  </si>
+  <si>
+    <t>If selected to join queue shall update the json with message type on that user Id and refer the player to PageManager with type 'JoinQueue'</t>
+  </si>
+  <si>
+    <t>Once a player enters loggined their name shall be added to the list of players in lobby</t>
+  </si>
+  <si>
+    <t>If user select to challenge shall update the json type for  the challenger "req_challenge" and refer to page manager</t>
+  </si>
+  <si>
+    <t>If select to view a match shall update the json along with the action</t>
+  </si>
+  <si>
+    <t>If a player is active shall be added to list of players for challenge</t>
+  </si>
+  <si>
+    <t>Players in a challenge cannot be challenged until they have completed their current match</t>
+  </si>
+  <si>
+    <t>If a player is not online, they won't be in the lobby list</t>
+  </si>
+  <si>
+    <t>If a player is online, status shall show as active</t>
+  </si>
+  <si>
+    <t>If player is in challenge, status shall show as in challenge</t>
+  </si>
+  <si>
+    <t>If player is in queue , status shall as busy</t>
+  </si>
+  <si>
+    <t>If player views a match,  shall redirect through the updated json</t>
+  </si>
+  <si>
+    <t>shall display number of players currently logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">players shall have unique userIDs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">default shall have 2 bots to be played against </t>
+  </si>
+  <si>
+    <t>shall update html and send to Page manager JSON for player request</t>
+  </si>
+  <si>
+    <t>shall try to reconnect if matchmaking failed in challenge mode</t>
+  </si>
+  <si>
+    <t>shall have a button to request a checkers game between two bots</t>
+  </si>
+  <si>
+    <t>shall have a button for the player to play aganist a bot</t>
+  </si>
+  <si>
+    <t>There shall be a scroll controll in the lobby to preserve height of the div in index page</t>
+  </si>
+  <si>
+    <t>The join game front end shall show the user in the lobby menu with different action buttons and options</t>
+  </si>
+  <si>
+    <t>There shall be a color indicator to show the status of the player</t>
+  </si>
+  <si>
+    <t>A function with the parameter of a player's info shall create a list element with the requirements T2_... and append to the id "lobby_list_items"</t>
+  </si>
+  <si>
+    <t>Create a paragraph element with the id "UID{player_id}" and the innerText of "{player_username} - (ELO: (player_elo})" and T2_35</t>
+  </si>
+  <si>
+    <t>A span element shall have the class "status free" if the player_status is ONLINE else it will be initialized with "status busy"</t>
+  </si>
+  <si>
+    <t>A challange button shall have the id "chall_btn-{player_id}", an onclick function that calls T2_37, and the inner text "Challenge"</t>
+  </si>
+  <si>
+    <t>A challenge function shall take in the parameters of the challenged player and current player then send it to PageManager with the correct format</t>
+  </si>
+  <si>
+    <t>A view button shall have the id "view_btn-{player_id}", an onclick function that call T2_39, and inner text of "view match"</t>
+  </si>
+  <si>
+    <t>a view match function shall take in the requested player's info and send to page manager in the corrent JSON format</t>
+  </si>
+  <si>
+    <t>getActivePlayer() method from PageManager</t>
+  </si>
+  <si>
+    <t>displayJoinGame(player) , updateJoinGameList(data)</t>
+  </si>
+  <si>
+    <t>sendMessage({'action':typeEvent})</t>
+  </si>
+  <si>
+    <t>Human players  shall have a "name, elo" tied to them</t>
+  </si>
+  <si>
+    <t>displayJoinGame(player)</t>
+  </si>
+  <si>
+    <t>sendMessage({action:'joinQueue', playerClientId: globalClientID})</t>
+  </si>
+  <si>
+    <t>sendMessage({ action: "challengePlayer", "opponentClientId": player_info.ClientID });</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>updateStatus(playerID, status)</t>
+  </si>
+  <si>
+    <t>globalClientID</t>
+  </si>
+  <si>
+    <t>sendMessage({'action':'challengeBot', 'botId': 0/1})</t>
+  </si>
+  <si>
+    <t>SwapToPage()</t>
+  </si>
+  <si>
+    <t>not implemented</t>
+  </si>
+  <si>
+    <t>The color status indicator shall be red to show that the player is busy</t>
+  </si>
+  <si>
+    <t>The color status indicator shall be green to show that the player is idle</t>
+  </si>
+  <si>
+    <t>case loginSuccessful; swapToPage("join_game");</t>
+  </si>
+  <si>
+    <t>Interface/Team2-Join_Game.md</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,13 +906,25 @@
       <color theme="1"/>
       <name val="Times"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -594,10 +954,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -626,8 +987,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -960,33 +1325,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:E90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="36.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="8.81640625" style="3"/>
-    <col min="17" max="17" width="8.81640625" style="12"/>
-    <col min="18" max="18" width="8.81640625" style="3"/>
-    <col min="19" max="19" width="36.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="36.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="8.77734375" style="3"/>
+    <col min="17" max="17" width="8.77734375" style="12"/>
+    <col min="18" max="18" width="8.77734375" style="3"/>
+    <col min="19" max="19" width="36.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F2" s="9" t="s">
         <v>49</v>
       </c>
@@ -1024,7 +1389,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1067,7 +1432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1075,27 +1440,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1474,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="78" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1123,7 +1488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1151,7 +1516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1165,7 +1530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1179,7 +1544,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -1193,7 +1558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1207,7 +1572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -1221,7 +1586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -1235,7 +1600,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1249,7 +1614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
@@ -1263,7 +1628,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
@@ -1277,7 +1642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
@@ -1291,7 +1656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1307,7 +1672,7 @@
       <c r="F24" s="10"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1323,7 +1688,7 @@
       <c r="F25" s="10"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1339,7 +1704,7 @@
       <c r="F26" s="10"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -1355,7 +1720,7 @@
       <c r="F27" s="10"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -1373,7 +1738,7 @@
       </c>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -1389,7 +1754,7 @@
       <c r="F29" s="10"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1405,7 +1770,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1423,7 +1788,7 @@
       </c>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -1441,7 +1806,7 @@
       </c>
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
@@ -1455,7 +1820,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -1469,7 +1834,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>123</v>
       </c>
@@ -1483,7 +1848,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
@@ -1497,7 +1862,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>109</v>
       </c>
@@ -1511,7 +1876,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>110</v>
       </c>
@@ -1525,7 +1890,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>111</v>
       </c>
@@ -1539,7 +1904,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>112</v>
       </c>
@@ -1553,7 +1918,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>113</v>
       </c>
@@ -1567,7 +1932,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -1581,7 +1946,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
@@ -1595,7 +1960,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>156</v>
       </c>
@@ -1609,7 +1974,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>124</v>
       </c>
@@ -1623,7 +1988,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>125</v>
       </c>
@@ -1637,7 +2002,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>126</v>
       </c>
@@ -1651,7 +2016,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>127</v>
       </c>
@@ -1665,7 +2030,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>128</v>
       </c>
@@ -1679,7 +2044,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>129</v>
       </c>
@@ -1693,7 +2058,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>130</v>
       </c>
@@ -1707,7 +2072,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>131</v>
       </c>
@@ -1721,7 +2086,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>132</v>
       </c>
@@ -1735,7 +2100,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>133</v>
       </c>
@@ -1749,7 +2114,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>134</v>
       </c>
@@ -1763,7 +2128,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>135</v>
       </c>
@@ -1775,6 +2140,485 @@
       </c>
       <c r="D56" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C65" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C68" t="s">
+        <v>237</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C73" t="s">
+        <v>242</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" t="s">
+        <v>243</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" t="s">
+        <v>244</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" t="s">
+        <v>245</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" t="s">
+        <v>246</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C78" t="s">
+        <v>247</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added login signup requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uta\SPring 2025\fundamental\projectFinal\cse3310-sp25-004\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdubc\Documents\cse3310-sp25-004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F121F39-4C40-47D8-86E9-FDB2C932ED91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B9412A-E197-4A3F-B1D3-1D7DFB04D656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="320">
   <si>
     <t>Tested By</t>
   </si>
@@ -863,6 +863,141 @@
   </si>
   <si>
     <t>Interface/Team2-Join_Game.md</t>
+  </si>
+  <si>
+    <t>System shall have a username box for the returning user to enter thier unique identifier</t>
+  </si>
+  <si>
+    <t>System shall have a password box for the returning user to enter their created password.</t>
+  </si>
+  <si>
+    <t>System shall have a login button for directing returning users to login page.</t>
+  </si>
+  <si>
+    <t>System shall have a sign up button for directing new users to new account page.</t>
+  </si>
+  <si>
+    <t>System shall have a game title (logo)</t>
+  </si>
+  <si>
+    <t>System shall have a sign up information input to create new accounts for new users.</t>
+  </si>
+  <si>
+    <t>System users shall have a unique username with at least 4 characters.</t>
+  </si>
+  <si>
+    <t>System users shall have a password with at least 6 unique characters.</t>
+  </si>
+  <si>
+    <t>System shall display a message if no account is found matching the entered username.</t>
+  </si>
+  <si>
+    <t>System will comunicate with Page Manager to send data to database</t>
+  </si>
+  <si>
+    <t>System shall have a username box for the new user to enter thier unique identifier</t>
+  </si>
+  <si>
+    <t>System shall have a password box for the new user to enter their created password.</t>
+  </si>
+  <si>
+    <t>System shall have a functioning button to log the user in using their entered credentials.</t>
+  </si>
+  <si>
+    <t>System shall have a functioning button to create a user account using their entered credentials.</t>
+  </si>
+  <si>
+    <t>System shall have a function to show the signup page and simultaneuously hide the login screen upon click. Function for Requirement(4)</t>
+  </si>
+  <si>
+    <t>System shall have a function to show the login page and simultaneuously hide the signup screen upon click. Function for Requirement(3)</t>
+  </si>
+  <si>
+    <t>LS_01</t>
+  </si>
+  <si>
+    <t>LS_02</t>
+  </si>
+  <si>
+    <t>LS_03</t>
+  </si>
+  <si>
+    <t>LS_04</t>
+  </si>
+  <si>
+    <t>LS_05</t>
+  </si>
+  <si>
+    <t>LS_06</t>
+  </si>
+  <si>
+    <t>LS_07</t>
+  </si>
+  <si>
+    <t>LS_08</t>
+  </si>
+  <si>
+    <t>LS_09</t>
+  </si>
+  <si>
+    <t>LS_10</t>
+  </si>
+  <si>
+    <t>LS_11</t>
+  </si>
+  <si>
+    <t>LS_12</t>
+  </si>
+  <si>
+    <t>LS_13</t>
+  </si>
+  <si>
+    <t>LS_14</t>
+  </si>
+  <si>
+    <t>LS_15</t>
+  </si>
+  <si>
+    <t>LS_16</t>
+  </si>
+  <si>
+    <t>01 - Login/Signup</t>
+  </si>
+  <si>
+    <t>1 - Login/Signup</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>btn</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>new_account</t>
+  </si>
+  <si>
+    <t>uniqueUser, span</t>
+  </si>
+  <si>
+    <t>uniquePass, span</t>
+  </si>
+  <si>
+    <t>span</t>
+  </si>
+  <si>
+    <t>sendInfo</t>
+  </si>
+  <si>
+    <t>login (id)</t>
+  </si>
+  <si>
+    <t>new_account (id)</t>
+  </si>
+  <si>
+    <t>auth.js</t>
   </si>
 </sst>
 </file>
@@ -958,7 +1093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -989,6 +1124,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1325,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S90"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:E90"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2621,6 +2759,233 @@
         <v>265</v>
       </c>
     </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C91" t="s">
+        <v>275</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C92" t="s">
+        <v>276</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C93" t="s">
+        <v>277</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C94" t="s">
+        <v>278</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C95" t="s">
+        <v>279</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C96" t="s">
+        <v>280</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C97" t="s">
+        <v>281</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C98" t="s">
+        <v>282</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C99" t="s">
+        <v>283</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C100" t="s">
+        <v>284</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C101" t="s">
+        <v>285</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C102" t="s">
+        <v>286</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C103" t="s">
+        <v>287</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C104" t="s">
+        <v>288</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C107" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added team 6 to final req xcel file
</commit_message>
<xml_diff>
--- a/FinalRequirements.xlsx
+++ b/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdubc\Documents\cse3310-sp25-004\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taffy\Documents\School\CSE 3310 projects\project2\cse3310-sp25-004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B9412A-E197-4A3F-B1D3-1D7DFB04D656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84C46B8-852D-4F7F-9695-046B4CFE9FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="366">
   <si>
     <t>Tested By</t>
   </si>
@@ -998,6 +998,144 @@
   </si>
   <si>
     <t>auth.js</t>
+  </si>
+  <si>
+    <t>DB_1</t>
+  </si>
+  <si>
+    <t>6 - Database</t>
+  </si>
+  <si>
+    <t>The database shall ensure that each username is unique and associated with a UUID.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initializeDatabase() </t>
+  </si>
+  <si>
+    <t>DB_2</t>
+  </si>
+  <si>
+    <t>The database shall generate a UUID for each new user record upon creation.</t>
+  </si>
+  <si>
+    <t>DB_3</t>
+  </si>
+  <si>
+    <t>The database shall provide an interface that allows the page manager to request and retrieve stored user information by username, UUID, or other attributes.</t>
+  </si>
+  <si>
+    <t>getPlayer(String username, String password)</t>
+  </si>
+  <si>
+    <t>DB_4</t>
+  </si>
+  <si>
+    <t>The database shall support deletion of user records manually if needed.</t>
+  </si>
+  <si>
+    <t>DB_5</t>
+  </si>
+  <si>
+    <t>The database shall maintain data and value ranges for all fields to maintain consistency.</t>
+  </si>
+  <si>
+    <t>DB_6</t>
+  </si>
+  <si>
+    <t>The database shall respond to requests from page manager and deliver the requested information within a short span of time.</t>
+  </si>
+  <si>
+    <t>DB_7</t>
+  </si>
+  <si>
+    <t>The database shall ensure consistency by preventing duplicate names by using the UUID's.</t>
+  </si>
+  <si>
+    <t>addPlayer(String username, String password)</t>
+  </si>
+  <si>
+    <t>DB_8</t>
+  </si>
+  <si>
+    <t>The database shall be scalable to handle an increasing number of user records.</t>
+  </si>
+  <si>
+    <t>DB_9</t>
+  </si>
+  <si>
+    <t>The database shall support the insertion of new user records.</t>
+  </si>
+  <si>
+    <t>DB_10</t>
+  </si>
+  <si>
+    <t>The database shall support the update of a user's win count.</t>
+  </si>
+  <si>
+    <t>recordMatchResult(int winnerId, int loserId)</t>
+  </si>
+  <si>
+    <t>DB_11</t>
+  </si>
+  <si>
+    <t>The database shall support the update of a user's loss count.</t>
+  </si>
+  <si>
+    <t>DB_12</t>
+  </si>
+  <si>
+    <t>The database shall support the update of a user's total games played.</t>
+  </si>
+  <si>
+    <t>DB_13</t>
+  </si>
+  <si>
+    <t>The database shall support the update of a user's elo value.</t>
+  </si>
+  <si>
+    <t>DB_14</t>
+  </si>
+  <si>
+    <t>The database shall provide a user's elo value to pair up system upon request.</t>
+  </si>
+  <si>
+    <t>DB_15</t>
+  </si>
+  <si>
+    <t>The database shall store player's username.</t>
+  </si>
+  <si>
+    <t>updatePlayerStats(int playerId, int wins, int losses, int ELO, int gamesPlayed)</t>
+  </si>
+  <si>
+    <t>DB_16</t>
+  </si>
+  <si>
+    <t>The database shall store player's UUID.</t>
+  </si>
+  <si>
+    <t>DB_17</t>
+  </si>
+  <si>
+    <t>The database shall store player's wins.</t>
+  </si>
+  <si>
+    <t>DB_18</t>
+  </si>
+  <si>
+    <t>The database shall store player's losses.</t>
+  </si>
+  <si>
+    <t>DB_19</t>
+  </si>
+  <si>
+    <t>The database shall store player's total games.</t>
+  </si>
+  <si>
+    <t>DB_20</t>
+  </si>
+  <si>
+    <t>The database shall store player's elo.</t>
   </si>
 </sst>
 </file>
@@ -1463,33 +1601,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S107"/>
+  <dimension ref="A1:S126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="3"/>
-    <col min="2" max="2" width="36.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="8.77734375" style="3"/>
-    <col min="17" max="17" width="8.77734375" style="12"/>
-    <col min="18" max="18" width="8.77734375" style="3"/>
-    <col min="19" max="19" width="36.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="8.7109375" style="3"/>
+    <col min="2" max="2" width="36.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="8.7109375" style="3"/>
+    <col min="17" max="17" width="8.7109375" style="12"/>
+    <col min="18" max="18" width="8.7109375" style="3"/>
+    <col min="19" max="19" width="36.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" s="9" t="s">
         <v>49</v>
       </c>
@@ -1527,7 +1665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1547,7 +1685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1570,7 +1708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1578,27 +1716,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1612,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1626,7 +1764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1640,7 +1778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1654,7 +1792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1668,7 +1806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1682,7 +1820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -1696,7 +1834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1710,7 +1848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -1724,7 +1862,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
@@ -1738,7 +1876,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1752,7 +1890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
@@ -1766,7 +1904,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
@@ -1780,7 +1918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
@@ -1794,7 +1932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1810,7 +1948,7 @@
       <c r="F24" s="10"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1826,7 +1964,7 @@
       <c r="F25" s="10"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1842,7 +1980,7 @@
       <c r="F26" s="10"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -1858,7 +1996,7 @@
       <c r="F27" s="10"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -1876,7 +2014,7 @@
       </c>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -1892,7 +2030,7 @@
       <c r="F29" s="10"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1908,7 +2046,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1926,7 +2064,7 @@
       </c>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -1944,7 +2082,7 @@
       </c>
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
@@ -1958,7 +2096,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -1972,7 +2110,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>123</v>
       </c>
@@ -1986,7 +2124,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
@@ -2000,7 +2138,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>109</v>
       </c>
@@ -2014,7 +2152,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>110</v>
       </c>
@@ -2028,7 +2166,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>111</v>
       </c>
@@ -2042,7 +2180,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>112</v>
       </c>
@@ -2056,7 +2194,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>113</v>
       </c>
@@ -2070,7 +2208,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -2084,7 +2222,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
@@ -2098,7 +2236,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>156</v>
       </c>
@@ -2112,7 +2250,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>124</v>
       </c>
@@ -2126,7 +2264,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>125</v>
       </c>
@@ -2140,7 +2278,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>126</v>
       </c>
@@ -2154,7 +2292,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>127</v>
       </c>
@@ -2168,7 +2306,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>128</v>
       </c>
@@ -2182,7 +2320,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>129</v>
       </c>
@@ -2196,7 +2334,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>130</v>
       </c>
@@ -2210,7 +2348,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>131</v>
       </c>
@@ -2224,7 +2362,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>132</v>
       </c>
@@ -2238,7 +2376,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>133</v>
       </c>
@@ -2252,7 +2390,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>134</v>
       </c>
@@ -2266,7 +2404,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>135</v>
       </c>
@@ -2280,7 +2418,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>159</v>
       </c>
@@ -2297,7 +2435,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>160</v>
       </c>
@@ -2311,7 +2449,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>161</v>
       </c>
@@ -2325,7 +2463,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>162</v>
       </c>
@@ -2339,7 +2477,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>163</v>
       </c>
@@ -2353,7 +2491,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>164</v>
       </c>
@@ -2367,7 +2505,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>165</v>
       </c>
@@ -2381,7 +2519,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>166</v>
       </c>
@@ -2395,7 +2533,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>167</v>
       </c>
@@ -2409,7 +2547,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>168</v>
       </c>
@@ -2423,7 +2561,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>169</v>
       </c>
@@ -2437,7 +2575,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>170</v>
       </c>
@@ -2451,7 +2589,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>171</v>
       </c>
@@ -2465,7 +2603,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>172</v>
       </c>
@@ -2479,7 +2617,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>173</v>
       </c>
@@ -2493,7 +2631,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>174</v>
       </c>
@@ -2507,7 +2645,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>175</v>
       </c>
@@ -2521,7 +2659,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>176</v>
       </c>
@@ -2535,7 +2673,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>177</v>
       </c>
@@ -2549,7 +2687,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>178</v>
       </c>
@@ -2563,7 +2701,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>179</v>
       </c>
@@ -2577,7 +2715,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>180</v>
       </c>
@@ -2591,7 +2729,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>181</v>
       </c>
@@ -2605,7 +2743,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>182</v>
       </c>
@@ -2619,7 +2757,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>183</v>
       </c>
@@ -2633,7 +2771,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>184</v>
       </c>
@@ -2647,7 +2785,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>185</v>
       </c>
@@ -2661,7 +2799,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>186</v>
       </c>
@@ -2675,7 +2813,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>187</v>
       </c>
@@ -2689,7 +2827,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>188</v>
       </c>
@@ -2703,7 +2841,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>189</v>
       </c>
@@ -2717,7 +2855,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>190</v>
       </c>
@@ -2731,7 +2869,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>191</v>
       </c>
@@ -2745,7 +2883,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>192</v>
       </c>
@@ -2759,7 +2897,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>291</v>
       </c>
@@ -2773,7 +2911,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>292</v>
       </c>
@@ -2787,7 +2925,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>293</v>
       </c>
@@ -2801,7 +2939,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>294</v>
       </c>
@@ -2815,7 +2953,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>295</v>
       </c>
@@ -2829,7 +2967,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>296</v>
       </c>
@@ -2843,7 +2981,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>297</v>
       </c>
@@ -2857,7 +2995,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>298</v>
       </c>
@@ -2871,7 +3009,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>299</v>
       </c>
@@ -2885,7 +3023,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>300</v>
       </c>
@@ -2899,7 +3037,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>301</v>
       </c>
@@ -2913,7 +3051,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>302</v>
       </c>
@@ -2927,7 +3065,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>303</v>
       </c>
@@ -2941,7 +3079,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>304</v>
       </c>
@@ -2955,7 +3093,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>305</v>
       </c>
@@ -2969,7 +3107,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>306</v>
       </c>
@@ -2983,8 +3121,285 @@
         <v>319</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C107" s="7"/>
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>355</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>